<commit_message>
Login y sing-up preparados quitar CORS
</commit_message>
<xml_diff>
--- a/Documentación/Documentación YouRights/Documentación.xlsx
+++ b/Documentación/Documentación YouRights/Documentación.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF46231-F2D0-4952-A940-43123E579621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62677AA0-30AD-4EDB-8AF7-38FDD58819B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="4178" windowWidth="18225" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3398" yWindow="4178" windowWidth="18225" windowHeight="11422" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Socios-Personal" sheetId="3" r:id="rId1"/>
     <sheet name="Gastos-Ingresos" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Personas Protestantes" sheetId="5" r:id="rId3"/>
     <sheet name="Merchandising" sheetId="1" r:id="rId4"/>
+    <sheet name="Contraseñas" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2D20A8B8-9A59-4156-8EA9-AD3500040345}">
@@ -43,7 +44,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -94,7 +95,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -118,7 +119,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -142,7 +143,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -166,7 +167,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -195,7 +196,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="149">
   <si>
     <t>Fecha revisión</t>
   </si>
@@ -636,6 +637,33 @@
   </si>
   <si>
     <t>Román Rodriguez</t>
+  </si>
+  <si>
+    <t>Pruebas DB</t>
+  </si>
+  <si>
+    <t>Redes Sociales</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Relacionado al:</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Tus Derechos</t>
+  </si>
+  <si>
+    <t>tusderechos0000</t>
+  </si>
+  <si>
+    <t>Tel: 689782048</t>
   </si>
 </sst>
 </file>
@@ -646,7 +674,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,8 +765,23 @@
       <color rgb="FF222222"/>
       <name val="Droid Serif"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -763,6 +806,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -777,7 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,9 +873,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1107,11 +1164,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC681F9-A6CF-4A0D-BC77-4953A2588DD7}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="16.9296875" customWidth="1"/>
     <col min="3" max="4" width="12.46484375" customWidth="1"/>
@@ -1264,7 +1321,7 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="16.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -1520,10 +1577,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="24.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1791,7 +1848,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.06640625" bestFit="1" customWidth="1"/>
@@ -1991,4 +2048,76 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0E65B2-7D82-4470-A1B5-E3C3AB90E7B7}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.19921875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
+    <col min="8" max="8" width="14.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75">
+      <c r="A1" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="E1" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75">
+      <c r="A2" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>